<commit_message>
add tests for categoric
</commit_message>
<xml_diff>
--- a/Experiments/Experiment_Real_World/Hubway_LS_mod/Hubway Scaling Experiments.xlsx
+++ b/Experiments/Experiment_Real_World/Hubway_LS_mod/Hubway Scaling Experiments.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="28160" windowHeight="16820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="180" yWindow="620" windowWidth="28160" windowHeight="16820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary_hubway_lsmod" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
   <si>
     <t>seed</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Robust Dunn (2000)</t>
   </si>
   <si>
-    <t>Silhouette (2000</t>
-  </si>
-  <si>
     <t>Silhouette (5000)</t>
   </si>
   <si>
@@ -129,14 +126,30 @@
     <t>Geometric (90th perc.)</t>
   </si>
   <si>
-    <t>% of original</t>
+    <t>random_hubway_sample_seed1_obs_5001</t>
+  </si>
+  <si>
+    <t>Silhouette (2000)</t>
+  </si>
+  <si>
+    <t>% Improvement (divided by full search)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,15 +175,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -216,18 +235,28 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Hubway Scaling Experiments</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Results by Metric (Sample Size)</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -276,7 +305,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dunn (2000)</c:v>
+                  <c:v>Silhouette (2000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -329,13 +358,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>26532.489769104</c:v>
+                  <c:v>2.947153129432222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12313.341983603</c:v>
+                  <c:v>1.184358524437777</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6847.483980368</c:v>
+                  <c:v>0.763028075981111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,7 +380,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Robust Dunn (2000)</c:v>
+                  <c:v>Dunn (2000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -404,13 +433,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>44936.408678649</c:v>
+                  <c:v>7.370136046973332</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15378.071713334</c:v>
+                  <c:v>3.420372773223056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10310.519581005</c:v>
+                  <c:v>1.902078883435556</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -426,7 +455,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Silhouette (2000</c:v>
+                  <c:v>Robust Dunn (2000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -479,13 +508,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10609.751265956</c:v>
+                  <c:v>12.48233574406917</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4263.690687976</c:v>
+                  <c:v>4.271686587037222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2746.901073532</c:v>
+                  <c:v>2.864033216945834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -553,11 +582,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>38.90299347670528</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>65000.95093518</c:v>
+                  <c:v>18.05581970421667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33935.151388683</c:v>
+                  <c:v>9.426430941300832</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -626,7 +658,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="2">
-                  <c:v>136180.490824347</c:v>
+                  <c:v>37.82791411787417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,7 +727,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="2">
-                  <c:v>104777.631788447</c:v>
+                  <c:v>29.10489771901306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,7 +735,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -713,11 +744,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2083225840"/>
-        <c:axId val="-2083170368"/>
+        <c:axId val="-2125628640"/>
+        <c:axId val="-2050915120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2083225840"/>
+        <c:axId val="-2125628640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,7 +791,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083170368"/>
+        <c:crossAx val="-2050915120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -768,7 +799,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2083170368"/>
+        <c:axId val="-2050915120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -788,6 +819,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime (hours)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -819,7 +906,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083225840"/>
+        <c:crossAx val="-2125628640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -941,7 +1028,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1049,11 +1136,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1064,11 +1146,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1100,9 +1177,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1460,20 +1534,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>507246</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>26029</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>88017</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>528118</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>62871</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>113168</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>188612</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1754,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:P14"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2460,6 +2534,56 @@
       </c>
       <c r="P14" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>-10</v>
+      </c>
+      <c r="E15">
+        <v>0.74654702772046</v>
+      </c>
+      <c r="F15">
+        <v>-0.23866194305353</v>
+      </c>
+      <c r="G15">
+        <v>-0.24437186583198101</v>
+      </c>
+      <c r="H15">
+        <v>-10</v>
+      </c>
+      <c r="I15">
+        <v>1.15713103537461E-2</v>
+      </c>
+      <c r="J15">
+        <v>-10</v>
+      </c>
+      <c r="K15">
+        <v>-10</v>
+      </c>
+      <c r="L15">
+        <v>140050.77651613901</v>
+      </c>
+      <c r="M15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2471,8 +2595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="101" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2498,22 +2622,22 @@
         <v>15</v>
       </c>
       <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
-      </c>
-      <c r="O1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
@@ -2527,16 +2651,19 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2">
-        <v>26532.489769103999</v>
+        <v>2.9471531294322224</v>
       </c>
       <c r="K2">
-        <v>44936.408678649001</v>
+        <v>7.3701360469733324</v>
       </c>
       <c r="L2">
-        <v>10609.751265956</v>
+        <v>12.482335744069166</v>
+      </c>
+      <c r="M2">
+        <v>38.902993476705284</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
@@ -2550,19 +2677,19 @@
         <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3">
-        <v>12313.341983603001</v>
+        <v>1.1843585244377777</v>
       </c>
       <c r="K3">
-        <v>15378.071713334</v>
+        <v>3.4203727732230558</v>
       </c>
       <c r="L3">
-        <v>4263.6906879759999</v>
+        <v>4.2716865870372223</v>
       </c>
       <c r="M3">
-        <v>65000.950935180001</v>
+        <v>18.055819704216667</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
@@ -2576,25 +2703,25 @@
         <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4">
-        <v>6847.4839803679997</v>
+        <v>0.76302807598111111</v>
       </c>
       <c r="K4">
-        <v>10310.519581005001</v>
+        <v>1.9020788834355555</v>
       </c>
       <c r="L4">
-        <v>2746.9010735319998</v>
+        <v>2.8640332169458338</v>
       </c>
       <c r="M4">
-        <v>33935.151388683</v>
+        <v>9.4264309413008327</v>
       </c>
       <c r="N4">
-        <v>136180.49082434701</v>
+        <v>37.827914117874165</v>
       </c>
       <c r="O4">
-        <v>104777.631788447</v>
+        <v>29.10489771901306</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
@@ -2618,9 +2745,15 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
+      <c r="I6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -2633,17 +2766,21 @@
         <v>18</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J7">
         <f>J2/J$2</f>
         <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:L7" si="0">K2/K$2</f>
+        <f t="shared" ref="K7:O7" si="0">K2/K$2</f>
         <v>1</v>
       </c>
       <c r="L7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2659,19 +2796,23 @@
         <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8">
-        <f>J3/J$2</f>
-        <v>0.46408543226657095</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ref="K8:L8" si="1">K3/K$2</f>
-        <v>0.34221852981857687</v>
-      </c>
-      <c r="L8">
+        <v>31</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:O9" si="1">J3/J$2</f>
+        <v>0.40186528233297053</v>
+      </c>
+      <c r="K8" s="3">
         <f t="shared" si="1"/>
-        <v>0.40186528233297059</v>
+        <v>0.46408543226657101</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.34221852981857692</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.46412417376128928</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -2685,19 +2826,23 @@
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9">
-        <f>J4/J$2</f>
+        <v>32</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.25890343747700367</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
         <v>0.25807920929989825</v>
       </c>
-      <c r="K9">
-        <f t="shared" ref="K9:L9" si="2">K4/K$2</f>
-        <v>0.22944689805404769</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0.25890343747700367</v>
+      <c r="L9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.22944689805404772</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.24230605665204874</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -2756,6 +2901,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I6:O6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>